<commit_message>
integrating unified instruments distribution
</commit_message>
<xml_diff>
--- a/data/reference_reports/AO_TPT_V5.0_BIL Invest - Bonds USD Corporate Investment Grade - P USD CAP_LU1689732417_20201231.xlsx
+++ b/data/reference_reports/AO_TPT_V5.0_BIL Invest - Bonds USD Corporate Investment Grade - P USD CAP_LU1689732417_20201231.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugo Durand\Workspace\data\BIL MI 20201231\Final reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugo Durand\Workspace\TPT_generator\data\reference_reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5557A5AE-BBE6-40F8-9EB3-4BC0B2922F6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AC3BBE-D68B-4771-A08F-1B98228ACD6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="663" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5550,9 +5550,9 @@
   </sheetPr>
   <dimension ref="A1:EK162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EA1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="EL1" sqref="EL1:EL1048576"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
53 ok 59 WIP
</commit_message>
<xml_diff>
--- a/data/reference_reports/AO_TPT_V5.0_BIL Invest - Bonds USD Corporate Investment Grade - P USD CAP_LU1689732417_20201231.xlsx
+++ b/data/reference_reports/AO_TPT_V5.0_BIL Invest - Bonds USD Corporate Investment Grade - P USD CAP_LU1689732417_20201231.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugo Durand\Workspace\TPT_generator\data\reference_reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AC3BBE-D68B-4771-A08F-1B98228ACD6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071C2764-C367-4BFF-8906-6C0BAB2AB80B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="663" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Methodology!$B$4:$C$157</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Production Assumption'!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$A$1:$EK$161</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$A$1:$EK$157</definedName>
     <definedName name="NAV" localSheetId="2">#REF!</definedName>
     <definedName name="NAV">SCR!$B$10</definedName>
     <definedName name="ReportingDate" localSheetId="1">SCR!$C$6</definedName>
@@ -5545,14 +5545,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1">
+  <sheetPr codeName="Sheet1" filterMode="1">
     <tabColor theme="5"/>
   </sheetPr>
   <dimension ref="A1:EK162"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AW1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="BJ161" sqref="BJ161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18" defaultRowHeight="15"/>
@@ -7477,7 +7477,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="9" spans="1:141">
+    <row r="9" spans="1:141" hidden="1">
       <c r="A9" s="68" t="s">
         <v>354</v>
       </c>
@@ -7721,7 +7721,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="10" spans="1:141">
+    <row r="10" spans="1:141" hidden="1">
       <c r="A10" s="68" t="s">
         <v>354</v>
       </c>
@@ -7969,7 +7969,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="11" spans="1:141">
+    <row r="11" spans="1:141" hidden="1">
       <c r="A11" s="68" t="s">
         <v>354</v>
       </c>
@@ -8217,7 +8217,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="12" spans="1:141">
+    <row r="12" spans="1:141" hidden="1">
       <c r="A12" s="68" t="s">
         <v>354</v>
       </c>
@@ -8465,7 +8465,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="13" spans="1:141">
+    <row r="13" spans="1:141" hidden="1">
       <c r="A13" s="68" t="s">
         <v>354</v>
       </c>
@@ -8713,7 +8713,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="14" spans="1:141">
+    <row r="14" spans="1:141" hidden="1">
       <c r="A14" s="68" t="s">
         <v>354</v>
       </c>
@@ -8957,7 +8957,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="15" spans="1:141">
+    <row r="15" spans="1:141" hidden="1">
       <c r="A15" s="68" t="s">
         <v>354</v>
       </c>
@@ -9201,7 +9201,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="16" spans="1:141">
+    <row r="16" spans="1:141" hidden="1">
       <c r="A16" s="68" t="s">
         <v>354</v>
       </c>
@@ -9449,7 +9449,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="17" spans="1:141">
+    <row r="17" spans="1:141" hidden="1">
       <c r="A17" s="68" t="s">
         <v>354</v>
       </c>
@@ -9693,7 +9693,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="18" spans="1:141">
+    <row r="18" spans="1:141" hidden="1">
       <c r="A18" s="68" t="s">
         <v>354</v>
       </c>
@@ -9941,7 +9941,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="19" spans="1:141">
+    <row r="19" spans="1:141" hidden="1">
       <c r="A19" s="68" t="s">
         <v>354</v>
       </c>
@@ -10189,7 +10189,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="20" spans="1:141">
+    <row r="20" spans="1:141" hidden="1">
       <c r="A20" s="68" t="s">
         <v>354</v>
       </c>
@@ -10437,7 +10437,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="21" spans="1:141">
+    <row r="21" spans="1:141" hidden="1">
       <c r="A21" s="68" t="s">
         <v>354</v>
       </c>
@@ -10685,7 +10685,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="22" spans="1:141">
+    <row r="22" spans="1:141" hidden="1">
       <c r="A22" s="68" t="s">
         <v>354</v>
       </c>
@@ -11098,7 +11098,7 @@
         <v>771</v>
       </c>
       <c r="BJ23" s="68">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BL23" s="68"/>
       <c r="BM23" s="68"/>
@@ -11193,7 +11193,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="24" spans="1:141">
+    <row r="24" spans="1:141" hidden="1">
       <c r="A24" s="68" t="s">
         <v>354</v>
       </c>
@@ -11441,7 +11441,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="25" spans="1:141">
+    <row r="25" spans="1:141" hidden="1">
       <c r="A25" s="68" t="s">
         <v>354</v>
       </c>
@@ -11689,7 +11689,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="26" spans="1:141">
+    <row r="26" spans="1:141" hidden="1">
       <c r="A26" s="68" t="s">
         <v>354</v>
       </c>
@@ -11937,7 +11937,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="27" spans="1:141">
+    <row r="27" spans="1:141" hidden="1">
       <c r="A27" s="68" t="s">
         <v>354</v>
       </c>
@@ -12185,7 +12185,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="28" spans="1:141">
+    <row r="28" spans="1:141" hidden="1">
       <c r="A28" s="68" t="s">
         <v>354</v>
       </c>
@@ -12433,7 +12433,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="29" spans="1:141">
+    <row r="29" spans="1:141" hidden="1">
       <c r="A29" s="68" t="s">
         <v>354</v>
       </c>
@@ -12681,7 +12681,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="30" spans="1:141">
+    <row r="30" spans="1:141" hidden="1">
       <c r="A30" s="68" t="s">
         <v>354</v>
       </c>
@@ -12929,7 +12929,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="31" spans="1:141">
+    <row r="31" spans="1:141" hidden="1">
       <c r="A31" s="68" t="s">
         <v>354</v>
       </c>
@@ -13177,7 +13177,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="32" spans="1:141">
+    <row r="32" spans="1:141" hidden="1">
       <c r="A32" s="68" t="s">
         <v>354</v>
       </c>
@@ -13425,7 +13425,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="33" spans="1:141">
+    <row r="33" spans="1:141" hidden="1">
       <c r="A33" s="68" t="s">
         <v>354</v>
       </c>
@@ -13838,7 +13838,7 @@
         <v>700</v>
       </c>
       <c r="BJ34" s="68">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BL34" s="68"/>
       <c r="BM34" s="68"/>
@@ -13933,7 +13933,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="35" spans="1:141">
+    <row r="35" spans="1:141" hidden="1">
       <c r="A35" s="68" t="s">
         <v>354</v>
       </c>
@@ -14342,7 +14342,7 @@
         <v>835</v>
       </c>
       <c r="BJ36" s="68">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BL36" s="68"/>
       <c r="BM36" s="68"/>
@@ -14434,7 +14434,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="37" spans="1:141">
+    <row r="37" spans="1:141" hidden="1">
       <c r="A37" s="68" t="s">
         <v>354</v>
       </c>
@@ -14691,7 +14691,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="38" spans="1:141">
+    <row r="38" spans="1:141" hidden="1">
       <c r="A38" s="68" t="s">
         <v>354</v>
       </c>
@@ -15104,7 +15104,7 @@
         <v>700</v>
       </c>
       <c r="BJ39" s="68">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BL39" s="68"/>
       <c r="BM39" s="68"/>
@@ -15199,7 +15199,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="40" spans="1:141">
+    <row r="40" spans="1:141" hidden="1">
       <c r="A40" s="68" t="s">
         <v>354</v>
       </c>
@@ -15444,7 +15444,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="41" spans="1:141">
+    <row r="41" spans="1:141" hidden="1">
       <c r="A41" s="68" t="s">
         <v>354</v>
       </c>
@@ -15689,7 +15689,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="42" spans="1:141">
+    <row r="42" spans="1:141" hidden="1">
       <c r="A42" s="68" t="s">
         <v>354</v>
       </c>
@@ -15937,7 +15937,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="43" spans="1:141">
+    <row r="43" spans="1:141" hidden="1">
       <c r="A43" s="68" t="s">
         <v>354</v>
       </c>
@@ -16185,7 +16185,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="44" spans="1:141">
+    <row r="44" spans="1:141" hidden="1">
       <c r="A44" s="68" t="s">
         <v>354</v>
       </c>
@@ -16586,7 +16586,7 @@
         <v>771</v>
       </c>
       <c r="BJ45" s="68">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BL45" s="68"/>
       <c r="BM45" s="68"/>
@@ -16827,7 +16827,7 @@
         <v>771</v>
       </c>
       <c r="BJ46" s="68">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BL46" s="68"/>
       <c r="BM46" s="68"/>
@@ -16922,7 +16922,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="47" spans="1:141">
+    <row r="47" spans="1:141" hidden="1">
       <c r="A47" s="68" t="s">
         <v>354</v>
       </c>
@@ -17167,7 +17167,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="48" spans="1:141">
+    <row r="48" spans="1:141" hidden="1">
       <c r="A48" s="68" t="s">
         <v>354</v>
       </c>
@@ -17415,7 +17415,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="49" spans="1:141">
+    <row r="49" spans="1:141" hidden="1">
       <c r="A49" s="68" t="s">
         <v>354</v>
       </c>
@@ -17663,7 +17663,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:141">
+    <row r="50" spans="1:141" hidden="1">
       <c r="A50" s="68" t="s">
         <v>354</v>
       </c>
@@ -18057,7 +18057,7 @@
         <v>700</v>
       </c>
       <c r="BJ51" s="68">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BL51" s="68"/>
       <c r="BM51" s="68"/>
@@ -18152,7 +18152,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="52" spans="1:141">
+    <row r="52" spans="1:141" hidden="1">
       <c r="A52" s="68" t="s">
         <v>354</v>
       </c>
@@ -18397,7 +18397,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="53" spans="1:141">
+    <row r="53" spans="1:141" hidden="1">
       <c r="A53" s="68" t="s">
         <v>354</v>
       </c>
@@ -18645,7 +18645,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="54" spans="1:141">
+    <row r="54" spans="1:141" hidden="1">
       <c r="A54" s="68" t="s">
         <v>354</v>
       </c>
@@ -18890,7 +18890,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="55" spans="1:141">
+    <row r="55" spans="1:141" hidden="1">
       <c r="A55" s="68" t="s">
         <v>354</v>
       </c>
@@ -19138,7 +19138,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="56" spans="1:141">
+    <row r="56" spans="1:141" hidden="1">
       <c r="A56" s="68" t="s">
         <v>354</v>
       </c>
@@ -19379,7 +19379,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="57" spans="1:141">
+    <row r="57" spans="1:141" hidden="1">
       <c r="A57" s="68" t="s">
         <v>354</v>
       </c>
@@ -19627,7 +19627,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="58" spans="1:141">
+    <row r="58" spans="1:141" hidden="1">
       <c r="A58" s="68" t="s">
         <v>354</v>
       </c>
@@ -19875,7 +19875,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="59" spans="1:141">
+    <row r="59" spans="1:141" hidden="1">
       <c r="A59" s="68" t="s">
         <v>354</v>
       </c>
@@ -20276,7 +20276,7 @@
         <v>700</v>
       </c>
       <c r="BJ60" s="68">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BL60" s="68"/>
       <c r="BM60" s="68"/>
@@ -20524,7 +20524,7 @@
         <v>700</v>
       </c>
       <c r="BJ61" s="68">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BL61" s="68"/>
       <c r="BM61" s="68"/>
@@ -20772,7 +20772,7 @@
         <v>700</v>
       </c>
       <c r="BJ62" s="68">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BL62" s="68"/>
       <c r="BM62" s="68"/>
@@ -20867,7 +20867,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="63" spans="1:141">
+    <row r="63" spans="1:141" hidden="1">
       <c r="A63" s="68" t="s">
         <v>354</v>
       </c>
@@ -21112,7 +21112,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="64" spans="1:141">
+    <row r="64" spans="1:141" hidden="1">
       <c r="A64" s="68" t="s">
         <v>354</v>
       </c>
@@ -21360,7 +21360,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="65" spans="1:141">
+    <row r="65" spans="1:141" hidden="1">
       <c r="A65" s="68" t="s">
         <v>354</v>
       </c>
@@ -21608,7 +21608,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="66" spans="1:141">
+    <row r="66" spans="1:141" hidden="1">
       <c r="A66" s="68" t="s">
         <v>354</v>
       </c>
@@ -21853,7 +21853,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="67" spans="1:141">
+    <row r="67" spans="1:141" hidden="1">
       <c r="A67" s="68" t="s">
         <v>354</v>
       </c>
@@ -22254,7 +22254,7 @@
         <v>700</v>
       </c>
       <c r="BJ68" s="68">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BL68" s="68"/>
       <c r="BM68" s="68"/>
@@ -22349,7 +22349,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="69" spans="1:141">
+    <row r="69" spans="1:141" hidden="1">
       <c r="A69" s="68" t="s">
         <v>354</v>
       </c>
@@ -22590,7 +22590,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="70" spans="1:141">
+    <row r="70" spans="1:141" hidden="1">
       <c r="A70" s="68" t="s">
         <v>354</v>
       </c>
@@ -22838,7 +22838,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="71" spans="1:141">
+    <row r="71" spans="1:141" hidden="1">
       <c r="A71" s="68" t="s">
         <v>354</v>
       </c>
@@ -23086,7 +23086,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="72" spans="1:141">
+    <row r="72" spans="1:141" hidden="1">
       <c r="A72" s="68" t="s">
         <v>354</v>
       </c>
@@ -23334,7 +23334,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="73" spans="1:141">
+    <row r="73" spans="1:141" hidden="1">
       <c r="A73" s="68" t="s">
         <v>354</v>
       </c>
@@ -23579,7 +23579,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="74" spans="1:141">
+    <row r="74" spans="1:141" hidden="1">
       <c r="A74" s="68" t="s">
         <v>354</v>
       </c>
@@ -23824,7 +23824,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="75" spans="1:141">
+    <row r="75" spans="1:141" hidden="1">
       <c r="A75" s="68" t="s">
         <v>354</v>
       </c>
@@ -24072,7 +24072,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="76" spans="1:141">
+    <row r="76" spans="1:141" hidden="1">
       <c r="A76" s="68" t="s">
         <v>354</v>
       </c>
@@ -24320,7 +24320,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="77" spans="1:141">
+    <row r="77" spans="1:141" hidden="1">
       <c r="A77" s="68" t="s">
         <v>354</v>
       </c>
@@ -24721,7 +24721,7 @@
         <v>835</v>
       </c>
       <c r="BJ78" s="68">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BL78" s="68"/>
       <c r="BM78" s="68"/>
@@ -24813,7 +24813,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="79" spans="1:141">
+    <row r="79" spans="1:141" hidden="1">
       <c r="A79" s="68" t="s">
         <v>354</v>
       </c>
@@ -25211,7 +25211,7 @@
         <v>700</v>
       </c>
       <c r="BJ80" s="68">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BL80" s="68"/>
       <c r="BM80" s="68"/>
@@ -25306,7 +25306,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="81" spans="1:141">
+    <row r="81" spans="1:141" hidden="1">
       <c r="A81" s="68" t="s">
         <v>354</v>
       </c>
@@ -25554,7 +25554,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="82" spans="1:141">
+    <row r="82" spans="1:141" hidden="1">
       <c r="A82" s="68" t="s">
         <v>354</v>
       </c>
@@ -25798,7 +25798,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="83" spans="1:141">
+    <row r="83" spans="1:141" hidden="1">
       <c r="A83" s="68" t="s">
         <v>354</v>
       </c>
@@ -26043,7 +26043,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="84" spans="1:141">
+    <row r="84" spans="1:141" hidden="1">
       <c r="A84" s="68" t="s">
         <v>354</v>
       </c>
@@ -26291,7 +26291,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="85" spans="1:141">
+    <row r="85" spans="1:141" hidden="1">
       <c r="A85" s="68" t="s">
         <v>354</v>
       </c>
@@ -26692,7 +26692,7 @@
         <v>700</v>
       </c>
       <c r="BJ86" s="68">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BL86" s="68"/>
       <c r="BM86" s="68"/>
@@ -26787,7 +26787,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="87" spans="1:141">
+    <row r="87" spans="1:141" hidden="1">
       <c r="A87" s="68" t="s">
         <v>354</v>
       </c>
@@ -27035,7 +27035,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="88" spans="1:141">
+    <row r="88" spans="1:141" hidden="1">
       <c r="A88" s="68" t="s">
         <v>354</v>
       </c>
@@ -27283,7 +27283,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="89" spans="1:141">
+    <row r="89" spans="1:141" hidden="1">
       <c r="A89" s="68" t="s">
         <v>354</v>
       </c>
@@ -27531,7 +27531,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="90" spans="1:141">
+    <row r="90" spans="1:141" hidden="1">
       <c r="A90" s="68" t="s">
         <v>354</v>
       </c>
@@ -27779,7 +27779,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="91" spans="1:141">
+    <row r="91" spans="1:141" hidden="1">
       <c r="A91" s="68" t="s">
         <v>354</v>
       </c>
@@ -28027,7 +28027,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="92" spans="1:141">
+    <row r="92" spans="1:141" hidden="1">
       <c r="A92" s="68" t="s">
         <v>354</v>
       </c>
@@ -28272,7 +28272,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="93" spans="1:141">
+    <row r="93" spans="1:141" hidden="1">
       <c r="A93" s="68" t="s">
         <v>354</v>
       </c>
@@ -28520,7 +28520,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="94" spans="1:141">
+    <row r="94" spans="1:141" hidden="1">
       <c r="A94" s="68" t="s">
         <v>354</v>
       </c>
@@ -28761,7 +28761,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="95" spans="1:141">
+    <row r="95" spans="1:141" hidden="1">
       <c r="A95" s="68" t="s">
         <v>354</v>
       </c>
@@ -29009,7 +29009,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="96" spans="1:141">
+    <row r="96" spans="1:141" hidden="1">
       <c r="A96" s="68" t="s">
         <v>354</v>
       </c>
@@ -29257,7 +29257,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="97" spans="1:141">
+    <row r="97" spans="1:141" hidden="1">
       <c r="A97" s="68" t="s">
         <v>354</v>
       </c>
@@ -29654,7 +29654,7 @@
         <v>700</v>
       </c>
       <c r="BJ98" s="68">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BL98" s="68"/>
       <c r="BM98" s="68"/>
@@ -29749,7 +29749,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="99" spans="1:141">
+    <row r="99" spans="1:141" hidden="1">
       <c r="A99" s="68" t="s">
         <v>354</v>
       </c>
@@ -29997,7 +29997,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="100" spans="1:141">
+    <row r="100" spans="1:141" hidden="1">
       <c r="A100" s="68" t="s">
         <v>354</v>
       </c>
@@ -30242,7 +30242,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="101" spans="1:141">
+    <row r="101" spans="1:141" hidden="1">
       <c r="A101" s="68" t="s">
         <v>354</v>
       </c>
@@ -30490,7 +30490,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="102" spans="1:141">
+    <row r="102" spans="1:141" hidden="1">
       <c r="A102" s="68" t="s">
         <v>354</v>
       </c>
@@ -30734,7 +30734,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="103" spans="1:141">
+    <row r="103" spans="1:141" hidden="1">
       <c r="A103" s="68" t="s">
         <v>354</v>
       </c>
@@ -30982,7 +30982,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="104" spans="1:141">
+    <row r="104" spans="1:141" hidden="1">
       <c r="A104" s="68" t="s">
         <v>354</v>
       </c>
@@ -31379,7 +31379,7 @@
         <v>771</v>
       </c>
       <c r="BJ105" s="68">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BL105" s="68"/>
       <c r="BM105" s="68"/>
@@ -31474,7 +31474,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="106" spans="1:141">
+    <row r="106" spans="1:141" hidden="1">
       <c r="A106" s="68" t="s">
         <v>354</v>
       </c>
@@ -31719,7 +31719,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="107" spans="1:141">
+    <row r="107" spans="1:141" hidden="1">
       <c r="A107" s="68" t="s">
         <v>354</v>
       </c>
@@ -31967,7 +31967,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="108" spans="1:141">
+    <row r="108" spans="1:141" hidden="1">
       <c r="A108" s="68" t="s">
         <v>354</v>
       </c>
@@ -32215,7 +32215,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="109" spans="1:141">
+    <row r="109" spans="1:141" hidden="1">
       <c r="A109" s="68" t="s">
         <v>354</v>
       </c>
@@ -32608,7 +32608,7 @@
         <v>700</v>
       </c>
       <c r="BJ110" s="68">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BL110" s="68"/>
       <c r="BM110" s="68"/>
@@ -32703,7 +32703,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="111" spans="1:141">
+    <row r="111" spans="1:141" hidden="1">
       <c r="A111" s="68" t="s">
         <v>354</v>
       </c>
@@ -32951,7 +32951,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="112" spans="1:141">
+    <row r="112" spans="1:141" hidden="1">
       <c r="A112" s="68" t="s">
         <v>354</v>
       </c>
@@ -33199,7 +33199,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="113" spans="1:141">
+    <row r="113" spans="1:141" hidden="1">
       <c r="A113" s="68" t="s">
         <v>354</v>
       </c>
@@ -33447,7 +33447,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="114" spans="1:141">
+    <row r="114" spans="1:141" hidden="1">
       <c r="A114" s="68" t="s">
         <v>354</v>
       </c>
@@ -33695,7 +33695,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="115" spans="1:141">
+    <row r="115" spans="1:141" hidden="1">
       <c r="A115" s="68" t="s">
         <v>354</v>
       </c>
@@ -33936,7 +33936,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="116" spans="1:141">
+    <row r="116" spans="1:141" hidden="1">
       <c r="A116" s="68" t="s">
         <v>354</v>
       </c>
@@ -34180,7 +34180,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="117" spans="1:141">
+    <row r="117" spans="1:141" hidden="1">
       <c r="A117" s="68" t="s">
         <v>354</v>
       </c>
@@ -34428,7 +34428,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="118" spans="1:141">
+    <row r="118" spans="1:141" hidden="1">
       <c r="A118" s="68" t="s">
         <v>354</v>
       </c>
@@ -34672,7 +34672,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="119" spans="1:141">
+    <row r="119" spans="1:141" hidden="1">
       <c r="A119" s="68" t="s">
         <v>354</v>
       </c>
@@ -34920,7 +34920,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="120" spans="1:141">
+    <row r="120" spans="1:141" hidden="1">
       <c r="A120" s="68" t="s">
         <v>354</v>
       </c>
@@ -35168,7 +35168,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="121" spans="1:141">
+    <row r="121" spans="1:141" hidden="1">
       <c r="A121" s="68" t="s">
         <v>354</v>
       </c>
@@ -35412,7 +35412,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="122" spans="1:141">
+    <row r="122" spans="1:141" hidden="1">
       <c r="A122" s="68" t="s">
         <v>354</v>
       </c>
@@ -35656,7 +35656,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="123" spans="1:141">
+    <row r="123" spans="1:141" hidden="1">
       <c r="A123" s="68" t="s">
         <v>354</v>
       </c>
@@ -36053,7 +36053,7 @@
         <v>771</v>
       </c>
       <c r="BJ124" s="68">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BL124" s="68"/>
       <c r="BM124" s="68"/>
@@ -36148,7 +36148,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="125" spans="1:141">
+    <row r="125" spans="1:141" hidden="1">
       <c r="A125" s="68" t="s">
         <v>354</v>
       </c>
@@ -36392,7 +36392,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="126" spans="1:141">
+    <row r="126" spans="1:141" hidden="1">
       <c r="A126" s="68" t="s">
         <v>354</v>
       </c>
@@ -36640,7 +36640,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="127" spans="1:141">
+    <row r="127" spans="1:141" hidden="1">
       <c r="A127" s="68" t="s">
         <v>354</v>
       </c>
@@ -36884,7 +36884,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="128" spans="1:141">
+    <row r="128" spans="1:141" hidden="1">
       <c r="A128" s="68" t="s">
         <v>354</v>
       </c>
@@ -37132,7 +37132,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="129" spans="1:141">
+    <row r="129" spans="1:141" hidden="1">
       <c r="A129" s="68" t="s">
         <v>354</v>
       </c>
@@ -37380,7 +37380,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="130" spans="1:141">
+    <row r="130" spans="1:141" hidden="1">
       <c r="A130" s="68" t="s">
         <v>354</v>
       </c>
@@ -37628,7 +37628,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="131" spans="1:141">
+    <row r="131" spans="1:141" hidden="1">
       <c r="A131" s="68" t="s">
         <v>354</v>
       </c>
@@ -37873,7 +37873,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="132" spans="1:141">
+    <row r="132" spans="1:141" hidden="1">
       <c r="A132" s="68" t="s">
         <v>354</v>
       </c>
@@ -38118,7 +38118,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="133" spans="1:141">
+    <row r="133" spans="1:141" hidden="1">
       <c r="A133" s="68" t="s">
         <v>354</v>
       </c>
@@ -38366,7 +38366,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="134" spans="1:141">
+    <row r="134" spans="1:141" hidden="1">
       <c r="A134" s="68" t="s">
         <v>354</v>
       </c>
@@ -38614,7 +38614,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="135" spans="1:141">
+    <row r="135" spans="1:141" hidden="1">
       <c r="A135" s="68" t="s">
         <v>354</v>
       </c>
@@ -38862,7 +38862,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="136" spans="1:141">
+    <row r="136" spans="1:141" hidden="1">
       <c r="A136" s="68" t="s">
         <v>354</v>
       </c>
@@ -39110,7 +39110,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="137" spans="1:141">
+    <row r="137" spans="1:141" hidden="1">
       <c r="A137" s="68" t="s">
         <v>354</v>
       </c>
@@ -39523,7 +39523,7 @@
         <v>700</v>
       </c>
       <c r="BJ138" s="68">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BL138" s="68"/>
       <c r="BM138" s="68"/>
@@ -39615,7 +39615,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="139" spans="1:141">
+    <row r="139" spans="1:141" hidden="1">
       <c r="A139" s="68" t="s">
         <v>354</v>
       </c>
@@ -39863,7 +39863,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="140" spans="1:141">
+    <row r="140" spans="1:141" hidden="1">
       <c r="A140" s="68" t="s">
         <v>354</v>
       </c>
@@ -40111,7 +40111,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="141" spans="1:141">
+    <row r="141" spans="1:141" hidden="1">
       <c r="A141" s="68" t="s">
         <v>354</v>
       </c>
@@ -40359,7 +40359,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="142" spans="1:141">
+    <row r="142" spans="1:141" hidden="1">
       <c r="A142" s="68" t="s">
         <v>354</v>
       </c>
@@ -40607,7 +40607,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="143" spans="1:141">
+    <row r="143" spans="1:141" hidden="1">
       <c r="A143" s="68" t="s">
         <v>354</v>
       </c>
@@ -41001,7 +41001,7 @@
         <v>771</v>
       </c>
       <c r="BJ144" s="68">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BL144" s="68"/>
       <c r="BM144" s="68"/>
@@ -41096,7 +41096,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="145" spans="1:141">
+    <row r="145" spans="1:141" hidden="1">
       <c r="A145" s="68" t="s">
         <v>354</v>
       </c>
@@ -41344,7 +41344,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="146" spans="1:141">
+    <row r="146" spans="1:141" hidden="1">
       <c r="A146" s="68" t="s">
         <v>354</v>
       </c>
@@ -41589,7 +41589,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="147" spans="1:141">
+    <row r="147" spans="1:141" hidden="1">
       <c r="A147" s="68" t="s">
         <v>354</v>
       </c>
@@ -41837,7 +41837,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="148" spans="1:141">
+    <row r="148" spans="1:141" hidden="1">
       <c r="A148" s="68" t="s">
         <v>354</v>
       </c>
@@ -42085,7 +42085,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="149" spans="1:141">
+    <row r="149" spans="1:141" hidden="1">
       <c r="A149" s="68" t="s">
         <v>354</v>
       </c>
@@ -42341,7 +42341,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="150" spans="1:141">
+    <row r="150" spans="1:141" hidden="1">
       <c r="A150" s="68" t="s">
         <v>354</v>
       </c>
@@ -42598,7 +42598,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="151" spans="1:141">
+    <row r="151" spans="1:141" hidden="1">
       <c r="A151" s="68" t="s">
         <v>354</v>
       </c>
@@ -42851,7 +42851,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="152" spans="1:141">
+    <row r="152" spans="1:141" hidden="1">
       <c r="A152" s="68" t="s">
         <v>354</v>
       </c>
@@ -43269,7 +43269,7 @@
         <v>700</v>
       </c>
       <c r="BJ153" s="68">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BL153" s="68"/>
       <c r="BM153" s="68"/>
@@ -43364,7 +43364,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="154" spans="1:141">
+    <row r="154" spans="1:141" hidden="1">
       <c r="A154" s="68" t="s">
         <v>354</v>
       </c>
@@ -43785,7 +43785,7 @@
         <v>700</v>
       </c>
       <c r="BJ155" s="68">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BL155" s="68"/>
       <c r="BM155" s="68"/>
@@ -43880,7 +43880,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="156" spans="1:141">
+    <row r="156" spans="1:141" hidden="1">
       <c r="A156" s="68" t="s">
         <v>354</v>
       </c>
@@ -44124,7 +44124,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="157" spans="1:141">
+    <row r="157" spans="1:141" hidden="1">
       <c r="A157" s="68" t="s">
         <v>354</v>
       </c>
@@ -44401,6 +44401,13 @@
       <c r="CR162" s="68"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:EK157" xr:uid="{1343BF5B-2C66-41DF-8401-161EE5392CEA}">
+    <filterColumn colId="55">
+      <filters>
+        <filter val="K6419"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>